<commit_message>
Modificacion graficos en los excels
</commit_message>
<xml_diff>
--- a/Pruebas/Libro1.xlsx
+++ b/Pruebas/Libro1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="0" windowWidth="24960" windowHeight="15000" tabRatio="500"/>
+    <workbookView xWindow="285" yWindow="0" windowWidth="20640" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -130,13 +130,18 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-CL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -174,25 +179,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125.0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150.0</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -204,25 +209,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>419.0</c:v>
+                  <c:v>419</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>161.0</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>112.0</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>95.0</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>84.0</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>73.0</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>73.0</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -250,25 +255,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125.0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150.0</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -280,25 +285,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -326,25 +331,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125.0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150.0</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -356,25 +361,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4887.0</c:v>
+                  <c:v>4887</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7060.0</c:v>
+                  <c:v>7060</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10070.0</c:v>
+                  <c:v>10070</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10220.0</c:v>
+                  <c:v>10220</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9985.0</c:v>
+                  <c:v>9985</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9699.0</c:v>
+                  <c:v>9699</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9675.0</c:v>
+                  <c:v>9675</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -391,11 +396,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2056947432"/>
-        <c:axId val="2056950456"/>
+        <c:axId val="84910592"/>
+        <c:axId val="43478976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2056947432"/>
+        <c:axId val="84910592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -405,7 +410,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2056950456"/>
+        <c:crossAx val="43478976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -413,7 +418,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2056950456"/>
+        <c:axId val="43478976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -424,14 +429,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2056947432"/>
+        <c:crossAx val="84910592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -440,7 +444,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -449,7 +453,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-CL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -471,15 +475,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-ES"/>
-              <a:t>Gr</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="es-ES"/>
-              <a:t>á</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="es-ES"/>
-              <a:t>fico de Rendimiento (Peticiones/Seg)</a:t>
+              <a:t>Gráfico de Rendimiento (Peticiones/Seg)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -514,25 +510,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125.0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150.0</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -544,25 +540,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.421576696846204</c:v>
+                  <c:v>0.42157669684620402</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.96450737373545</c:v>
+                  <c:v>9.9645073737354508</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.6335481842477</c:v>
+                  <c:v>20.633548184247701</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.3278293939248</c:v>
+                  <c:v>30.327829393924802</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>40.0377498784568</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50.047187348071</c:v>
+                  <c:v>50.047187348070999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.4413960994556</c:v>
+                  <c:v>57.441396099455602</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -580,11 +576,11 @@
         <c:hiLowLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2057240888"/>
-        <c:axId val="2057243896"/>
+        <c:axId val="84911616"/>
+        <c:axId val="43481280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2057240888"/>
+        <c:axId val="84911616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -597,10 +593,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100"/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100"/>
+                  <a:rPr lang="es-ES" sz="1200"/>
                   <a:t>Nº de Usuarios</a:t>
                 </a:r>
               </a:p>
@@ -613,7 +609,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2057243896"/>
+        <c:crossAx val="43481280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -621,7 +617,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2057243896"/>
+        <c:axId val="43481280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -635,10 +631,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100"/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100"/>
+                  <a:rPr lang="es-ES" sz="1200"/>
                   <a:t>Rendimiento (Peticiones/Segundo)</a:t>
                 </a:r>
               </a:p>
@@ -651,7 +647,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2057240888"/>
+        <c:crossAx val="84911616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -662,7 +658,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -671,7 +667,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-CL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -728,25 +724,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125.0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150.0</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -758,25 +754,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>9075.19047619047</c:v>
+                  <c:v>9075.1904761904698</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1697.25333333333</c:v>
+                  <c:v>1697.2533333333299</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1555.45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1524.24031746031</c:v>
+                  <c:v>1524.2403174603101</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1511.09428571428</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1513.67219047619</c:v>
+                  <c:v>1513.6721904761901</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1505.24571428571</c:v>
+                  <c:v>1505.2457142857099</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -794,11 +790,11 @@
         <c:hiLowLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2078547160"/>
-        <c:axId val="2078550168"/>
+        <c:axId val="84912128"/>
+        <c:axId val="58720256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2078547160"/>
+        <c:axId val="84912128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,10 +807,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100"/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100"/>
+                  <a:rPr lang="es-ES" sz="1200"/>
                   <a:t>Nº de Usuarios</a:t>
                 </a:r>
               </a:p>
@@ -827,7 +823,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2078550168"/>
+        <c:crossAx val="58720256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -835,7 +831,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2078550168"/>
+        <c:axId val="58720256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -849,17 +845,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100"/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100"/>
+                  <a:rPr lang="es-ES" sz="1200"/>
                   <a:t>Tamaño</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+                  <a:rPr lang="es-ES" sz="1200" baseline="0"/>
                   <a:t> Medio de Respuesta (Bytes)</a:t>
                 </a:r>
-                <a:endParaRPr lang="es-ES" sz="1100"/>
+                <a:endParaRPr lang="es-ES" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -870,7 +866,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2078547160"/>
+        <c:crossAx val="84912128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -881,7 +877,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -890,7 +886,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-CL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -957,25 +953,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125.0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150.0</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -987,25 +983,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.73621955488527</c:v>
+                  <c:v>3.7362195548852699</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.5159114795869</c:v>
+                  <c:v>16.515911479586901</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.3422387921759</c:v>
+                  <c:v>31.342238792175898</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45.1434573274202</c:v>
+                  <c:v>45.143457327420201</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>59.0828272013612</c:v>
+                  <c:v>59.082827201361198</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>73.9795270511005</c:v>
+                  <c:v>73.979527051100504</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>84.4369290051697</c:v>
+                  <c:v>84.436929005169702</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1023,11 +1019,11 @@
         <c:hiLowLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2097492264"/>
-        <c:axId val="2079198344"/>
+        <c:axId val="84912640"/>
+        <c:axId val="58722560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2097492264"/>
+        <c:axId val="84912640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1040,15 +1036,15 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="600"/>
+                  <a:defRPr sz="700"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100" b="1" i="0" baseline="0">
+                  <a:rPr lang="es-ES" sz="1200" b="1" i="0" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
                   <a:t>Nº de Usuarios</a:t>
                 </a:r>
-                <a:endParaRPr lang="es-ES" sz="600">
+                <a:endParaRPr lang="es-ES" sz="700">
                   <a:effectLst/>
                 </a:endParaRPr>
               </a:p>
@@ -1061,7 +1057,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079198344"/>
+        <c:crossAx val="58722560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1069,7 +1065,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2079198344"/>
+        <c:axId val="58722560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1083,17 +1079,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100"/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100"/>
+                  <a:rPr lang="es-ES" sz="1200"/>
                   <a:t>Rendimiento</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+                  <a:rPr lang="es-ES" sz="1200" baseline="0"/>
                   <a:t> (Kb/Seg)</a:t>
                 </a:r>
-                <a:endParaRPr lang="es-ES" sz="1100"/>
+                <a:endParaRPr lang="es-ES" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1104,7 +1100,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097492264"/>
+        <c:crossAx val="84912640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1115,7 +1111,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1124,7 +1120,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-CL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1181,25 +1177,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125.0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150.0</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1211,25 +1207,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>419.0</c:v>
+                  <c:v>419</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>161.0</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>112.0</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>95.0</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>84.0</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>73.0</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>73.0</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1247,11 +1243,11 @@
         <c:hiLowLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2079249400"/>
-        <c:axId val="2097235416"/>
+        <c:axId val="84913664"/>
+        <c:axId val="58724288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2079249400"/>
+        <c:axId val="84913664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1264,10 +1260,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100"/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100"/>
+                  <a:rPr lang="es-ES" sz="1200"/>
                   <a:t>Nº de Usuarios</a:t>
                 </a:r>
               </a:p>
@@ -1280,7 +1276,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097235416"/>
+        <c:crossAx val="58724288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1288,7 +1284,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2097235416"/>
+        <c:axId val="58724288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1302,17 +1298,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100"/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100"/>
+                  <a:rPr lang="es-ES" sz="1200"/>
                   <a:t>Promedio</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+                  <a:rPr lang="es-ES" sz="1200" baseline="0"/>
                   <a:t> Respuesta (ms)</a:t>
                 </a:r>
-                <a:endParaRPr lang="es-ES" sz="1100"/>
+                <a:endParaRPr lang="es-ES" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1323,7 +1319,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079249400"/>
+        <c:crossAx val="84913664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1334,7 +1330,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1343,7 +1339,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-CL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1408,25 +1404,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125.0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150.0</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1438,25 +1434,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.274285714285714</c:v>
+                  <c:v>0.27428571428571402</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.282380952380952</c:v>
+                  <c:v>0.28238095238095201</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.283492063492063</c:v>
+                  <c:v>0.28349206349206302</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.284523809523809</c:v>
+                  <c:v>0.28452380952380901</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.284380952380952</c:v>
+                  <c:v>0.28438095238095201</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.284761904761904</c:v>
+                  <c:v>0.28476190476190399</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1474,11 +1470,11 @@
         <c:hiLowLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2079279304"/>
-        <c:axId val="2079246760"/>
+        <c:axId val="105021440"/>
+        <c:axId val="58726016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2079279304"/>
+        <c:axId val="105021440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1491,17 +1487,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100"/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100"/>
+                  <a:rPr lang="es-ES" sz="1200"/>
                   <a:t>Nº</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+                  <a:rPr lang="es-ES" sz="1200" baseline="0"/>
                   <a:t> de Usuarios</a:t>
                 </a:r>
-                <a:endParaRPr lang="es-ES" sz="1100"/>
+                <a:endParaRPr lang="es-ES" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1512,7 +1508,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079246760"/>
+        <c:crossAx val="58726016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1520,11 +1516,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2079246760"/>
+        <c:axId val="58726016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.3"/>
-          <c:min val="0.0"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1536,17 +1532,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100"/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100"/>
+                  <a:rPr lang="es-ES" sz="1200"/>
                   <a:t>% Peticiones</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+                  <a:rPr lang="es-ES" sz="1200" baseline="0"/>
                   <a:t> con Error</a:t>
                 </a:r>
-                <a:endParaRPr lang="es-ES" sz="1100"/>
+                <a:endParaRPr lang="es-ES" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1557,7 +1553,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079279304"/>
+        <c:crossAx val="105021440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1568,7 +1564,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1577,7 +1573,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-CL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1660,25 +1656,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125.0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150.0</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1690,25 +1686,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4887.0</c:v>
+                  <c:v>4887</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7060.0</c:v>
+                  <c:v>7060</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10070.0</c:v>
+                  <c:v>10070</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10220.0</c:v>
+                  <c:v>10220</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9985.0</c:v>
+                  <c:v>9985</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9699.0</c:v>
+                  <c:v>9699</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9675.0</c:v>
+                  <c:v>9675</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1726,11 +1722,11 @@
         <c:hiLowLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2079202600"/>
-        <c:axId val="2079205608"/>
+        <c:axId val="105021952"/>
+        <c:axId val="58727744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2079202600"/>
+        <c:axId val="105021952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1743,17 +1739,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES"/>
+                  <a:rPr lang="es-ES" sz="1200"/>
                   <a:t>Nº</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:rPr lang="es-ES" sz="1200" baseline="0"/>
                   <a:t> de Usuarios</a:t>
                 </a:r>
-                <a:endParaRPr lang="es-ES"/>
+                <a:endParaRPr lang="es-ES" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1764,7 +1760,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079205608"/>
+        <c:crossAx val="58727744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1772,7 +1768,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2079205608"/>
+        <c:axId val="58727744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1786,10 +1782,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES"/>
+                  <a:rPr lang="es-ES" sz="1200"/>
                   <a:t>Tiempo Maximo de Respuesta (ms)</a:t>
                 </a:r>
               </a:p>
@@ -1802,7 +1798,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079202600"/>
+        <c:crossAx val="105021952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1813,7 +1809,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1822,7 +1818,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-CL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1879,25 +1875,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125.0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150.0</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1909,25 +1905,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1945,11 +1941,11 @@
         <c:hiLowLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2097280440"/>
-        <c:axId val="2097285672"/>
+        <c:axId val="105022464"/>
+        <c:axId val="81429632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2097280440"/>
+        <c:axId val="105022464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1962,17 +1958,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100"/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100"/>
+                  <a:rPr lang="es-ES" sz="1200"/>
                   <a:t>Nº</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+                  <a:rPr lang="es-ES" sz="1200" baseline="0"/>
                   <a:t> de Usuarios</a:t>
                 </a:r>
-                <a:endParaRPr lang="es-ES" sz="1100"/>
+                <a:endParaRPr lang="es-ES" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1983,7 +1979,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097285672"/>
+        <c:crossAx val="81429632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1991,7 +1987,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2097285672"/>
+        <c:axId val="81429632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2005,10 +2001,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100"/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES" sz="1100"/>
+                  <a:rPr lang="es-ES" sz="1200"/>
                   <a:t>Tiempo Miniimo de Respuesta (ms)</a:t>
                 </a:r>
               </a:p>
@@ -2021,7 +2017,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097280440"/>
+        <c:crossAx val="105022464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2032,7 +2028,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2041,7 +2037,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-CL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2053,7 +2049,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2083,25 +2078,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125.0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150.0</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2113,25 +2108,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.274285714285714</c:v>
+                  <c:v>0.27428571428571402</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.282380952380952</c:v>
+                  <c:v>0.28238095238095201</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.283492063492063</c:v>
+                  <c:v>0.28349206349206302</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.284523809523809</c:v>
+                  <c:v>0.28452380952380901</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.284380952380952</c:v>
+                  <c:v>0.28438095238095201</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.284761904761904</c:v>
+                  <c:v>0.28476190476190399</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2148,11 +2143,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2097221224"/>
-        <c:axId val="2097237384"/>
+        <c:axId val="43183616"/>
+        <c:axId val="81431360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2097221224"/>
+        <c:axId val="43183616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2162,7 +2157,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097237384"/>
+        <c:crossAx val="81431360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2170,7 +2165,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2097237384"/>
+        <c:axId val="81431360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2181,14 +2176,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097221224"/>
+        <c:crossAx val="43183616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2197,7 +2191,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2806,22 +2800,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" customWidth="1"/>
+    <col min="3" max="3" width="10.125" customWidth="1"/>
+    <col min="4" max="4" width="10.625" customWidth="1"/>
+    <col min="5" max="5" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="12.125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2853,7 +2847,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2885,7 +2879,7 @@
         <v>9075.1904761904698</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>25</v>
       </c>
@@ -2917,7 +2911,7 @@
         <v>1697.2533333333299</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>50</v>
       </c>
@@ -2949,7 +2943,7 @@
         <v>1555.45</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>75</v>
       </c>
@@ -2981,7 +2975,7 @@
         <v>1524.2403174603101</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>100</v>
       </c>
@@ -3013,7 +3007,7 @@
         <v>1511.09428571428</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>125</v>
       </c>
@@ -3045,7 +3039,7 @@
         <v>1513.6721904761901</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>150</v>
       </c>

</xml_diff>